<commit_message>
updating files to latest legacy version (found in UW servers)
</commit_message>
<xml_diff>
--- a/ExcelSheets/ParkingGarage.xlsx
+++ b/ExcelSheets/ParkingGarage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zizhensong/Desktop/TS project/TS_MapWebApplication/TS_MapWebApplication/Excel sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zizhensong/Desktop/TS project/TS_MapWebApplication/TS_MapWebApplication/ExcelSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7D91D8-7E08-784D-B613-6963C0FB1544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A45C9-FA03-8247-9A6C-C87106350D46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5240" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{90F06434-E49C-2948-8A4A-D62E05310D02}"/>
+    <workbookView xWindow="-5240" yWindow="-21600" windowWidth="19160" windowHeight="21600" xr2:uid="{90F06434-E49C-2948-8A4A-D62E05310D02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Parking Garage</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Portage Bay Garage</t>
   </si>
   <si>
-    <t>South Campus Garage</t>
-  </si>
-  <si>
     <t>Padelford Garage</t>
   </si>
   <si>
@@ -66,37 +63,52 @@
     <t>4545 Garage</t>
   </si>
   <si>
-    <t>Tower Garage B</t>
-  </si>
-  <si>
-    <t>Tower Garage A</t>
-  </si>
-  <si>
     <t>PBG.png</t>
   </si>
   <si>
-    <t>SCG.png</t>
-  </si>
-  <si>
-    <t>PG.png</t>
-  </si>
-  <si>
     <t>MMG.png</t>
   </si>
   <si>
     <t>HG.png</t>
   </si>
   <si>
-    <t>4545G.png</t>
-  </si>
-  <si>
-    <t>TGA.png</t>
-  </si>
-  <si>
-    <t>TGB.png</t>
-  </si>
-  <si>
     <t>Icon</t>
+  </si>
+  <si>
+    <t>Tower Garage A (W46)</t>
+  </si>
+  <si>
+    <t>Tower Garage B (W45)</t>
+  </si>
+  <si>
+    <t>W45.png</t>
+  </si>
+  <si>
+    <t>W46.png</t>
+  </si>
+  <si>
+    <t>PDL.png</t>
+  </si>
+  <si>
+    <t>S1 Garage</t>
+  </si>
+  <si>
+    <t>S1.png</t>
+  </si>
+  <si>
+    <t>G4545.png</t>
+  </si>
+  <si>
+    <t>Cedar Garage East</t>
+  </si>
+  <si>
+    <t>Cedar Garage West</t>
+  </si>
+  <si>
+    <t>CGE.png</t>
+  </si>
+  <si>
+    <t>CGW.png</t>
   </si>
 </sst>
 </file>
@@ -448,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581F440B-BC39-7C40-A6F6-7B852607BFD0}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -471,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -499,12 +511,12 @@
         <v>-122.314004302024</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>47.649405864546402</v>
@@ -513,12 +525,12 @@
         <v>-122.309702038764</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>47.656629396441197</v>
@@ -527,12 +539,12 @@
         <v>-122.30310380458801</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>47.658204781419698</v>
@@ -541,12 +553,12 @@
         <v>-122.303409576416</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>47.659151434850301</v>
@@ -555,12 +567,12 @@
         <v>-122.304042577743</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>47.661460185549899</v>
@@ -569,12 +581,12 @@
         <v>-122.31259346008299</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>47.659967999975201</v>
@@ -583,12 +595,12 @@
         <v>-122.316445112228</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>47.660957977733098</v>
@@ -597,7 +609,35 @@
         <v>-122.315624356269</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>47.656922074768502</v>
+      </c>
+      <c r="C11">
+        <v>-122.315618991851</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>47.657446001010499</v>
+      </c>
+      <c r="C12">
+        <v>-122.316579222679</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>